<commit_message>
added retryListener and AnnotationTransformer
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="19440" windowHeight="11040"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="19440" windowHeight="11040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>username</t>
   </si>
@@ -409,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,17 +478,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -512,22 +511,6 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>